<commit_message>
Updating the Rmarkdown and more finessing of the Bayes model
</commit_message>
<xml_diff>
--- a/markdown/model_priors.xlsx
+++ b/markdown/model_priors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjjoy\Documents\SF_Rockfish_Removals\RockfishSportMort\markdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5430AF9-4FA8-4936-82D2-C2BFFE4EEE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21632C87-12C1-441C-8B60-2BCCE1D32C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3ADC3E42-4C40-4518-B615-B83EB1AEA46F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2142" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="85">
   <si>
     <t>Prior</t>
   </si>
@@ -414,7 +414,7 @@
     <t>HARVEST PROPORTION PRIORS:</t>
   </si>
   <si>
-    <t>fixed at 0 for WKMA??</t>
+    <t>offset to differentiates slope as a proportion of non-pelagics for harvests and as a proportion of non-pelagic, non-yelloweye for releases.</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -549,13 +549,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -564,8 +561,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7596,13 +7599,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EB88A8-0633-428F-BFF5-598E355F3438}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N59" sqref="N59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -7616,23 +7621,23 @@
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="20" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
       <c r="H1" s="8"/>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="20" t="s">
         <v>72</v>
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
       <c r="L1" s="8"/>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
       <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -7683,7 +7688,7 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -7727,7 +7732,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -7836,7 +7841,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>78</v>
       </c>
       <c r="C7" s="17" t="s">
@@ -7945,7 +7950,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C10" s="17" t="s">
@@ -8053,7 +8058,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="11" t="s">
         <v>80</v>
       </c>
@@ -8095,7 +8100,7 @@
       <c r="P13" s="12"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -8140,7 +8145,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -8244,7 +8249,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>78</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -8347,7 +8352,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="17" t="s">
@@ -8452,7 +8457,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="11" t="s">
         <v>80</v>
       </c>
@@ -8494,7 +8499,7 @@
       <c r="P25" s="12"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -8539,7 +8544,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="17" t="s">
@@ -8642,7 +8647,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="16" t="s">
         <v>78</v>
       </c>
       <c r="C31" s="17" t="s">
@@ -8751,7 +8756,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C34" s="17" t="s">
@@ -8854,7 +8859,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="11" t="s">
         <v>80</v>
       </c>
@@ -8896,7 +8901,7 @@
       <c r="P37" s="12"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="18" t="s">
         <v>34</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -9057,7 +9062,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="11" t="s">
         <v>80</v>
       </c>
@@ -9099,7 +9104,7 @@
       <c r="P43" s="12"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="18" t="s">
         <v>35</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -9298,46 +9303,56 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
+    <row r="50" spans="1:16" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="19"/>
       <c r="B50" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="12" t="s">
+      <c r="C50" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F50" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12" t="s">
+      <c r="F50" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J50" s="12">
+      <c r="J50" s="10">
         <v>0.01</v>
       </c>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
-      <c r="M50" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="N50" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="O50" s="12">
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N50" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="O50" s="10">
         <v>0.01</v>
       </c>
       <c r="P50" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B31:B33"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="A39:A43"/>
     <mergeCell ref="A45:A50"/>
@@ -9354,16 +9369,6 @@
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C16:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -9375,7 +9380,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9398,23 +9403,23 @@
       <c r="B1" s="15"/>
       <c r="C1" s="6"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="20" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
       <c r="H1" s="8"/>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="20" t="s">
         <v>72</v>
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
       <c r="L1" s="8"/>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
       <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -9464,7 +9469,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -9509,7 +9514,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C4" t="s">
@@ -9616,7 +9621,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>78</v>
       </c>
       <c r="C7" t="s">
@@ -9726,7 +9731,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C10" t="s">
@@ -9832,7 +9837,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="11" t="s">
         <v>80</v>
       </c>
@@ -9874,7 +9879,7 @@
       <c r="P13" s="12"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -9919,7 +9924,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C16" t="s">
@@ -10024,7 +10029,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>78</v>
       </c>
       <c r="C19" t="s">
@@ -10129,7 +10134,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C22" t="s">
@@ -10235,7 +10240,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="11" t="s">
         <v>80</v>
       </c>
@@ -10277,7 +10282,7 @@
       <c r="P25" s="12"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="18" t="s">
         <v>61</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -10322,7 +10327,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C28" t="s">
@@ -10395,9 +10400,6 @@
       <c r="O29" t="s">
         <v>54</v>
       </c>
-      <c r="P29" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
@@ -10435,7 +10437,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="16" t="s">
         <v>78</v>
       </c>
       <c r="C31" t="s">
@@ -10508,9 +10510,6 @@
       <c r="O32" t="s">
         <v>54</v>
       </c>
-      <c r="P32" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
@@ -10548,7 +10547,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C34" t="s">
@@ -10629,7 +10628,7 @@
         <v>21</v>
       </c>
       <c r="F36">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G36" t="s">
         <v>36</v>
@@ -10654,7 +10653,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="11" t="s">
         <v>80</v>
       </c>
@@ -10697,13 +10696,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="A27:A37"/>
     <mergeCell ref="A15:A25"/>
@@ -10712,6 +10704,13 @@
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
minor model fix, rmarkdown revision and prior excel sheet updated
</commit_message>
<xml_diff>
--- a/markdown/model_priors.xlsx
+++ b/markdown/model_priors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjjoy\Documents\Rockfish_SF_mortality\RockfishSportMort\markdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47319944-64E6-4CBF-B9A3-0DFED5800888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A46D1A-ED32-4FCC-8B3E-5DF82E16DD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="1065" windowWidth="17580" windowHeight="13560" activeTab="2" xr2:uid="{3ADC3E42-4C40-4518-B615-B83EB1AEA46F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3ADC3E42-4C40-4518-B615-B83EB1AEA46F}"/>
   </bookViews>
   <sheets>
     <sheet name="Coded" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="91">
   <si>
     <t>Prior</t>
   </si>
@@ -419,6 +419,45 @@
   <si>
     <t>fixed at 0 for CI and NGC; truncation on PWS areas</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hyperprior </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or SD</t>
+    </r>
+  </si>
+  <si>
+    <t>SD unif</t>
+  </si>
+  <si>
+    <t>(,50)</t>
+  </si>
+  <si>
+    <t>(,25)</t>
+  </si>
+  <si>
+    <t>fixed at 0 for NGC, PWSI, PWSO</t>
+  </si>
 </sst>
 </file>
 
@@ -515,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -555,13 +594,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -570,9 +606,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7602,8 +7642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EB88A8-0633-428F-BFF5-598E355F3438}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7624,23 +7664,23 @@
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="21" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="H1" s="8"/>
-      <c r="I1" s="17" t="s">
-        <v>72</v>
+      <c r="I1" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
       <c r="L1" s="8"/>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
       <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -7691,7 +7731,7 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -7714,7 +7754,7 @@
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J3" s="8">
         <v>0.1</v>
@@ -7735,7 +7775,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -7748,13 +7788,16 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G4">
         <v>0.1</v>
       </c>
+      <c r="H4" t="s">
+        <v>88</v>
+      </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J4">
         <v>0.1</v>
@@ -7789,7 +7832,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J5">
         <v>0.1</v>
@@ -7798,7 +7841,7 @@
         <v>5</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N5" t="s">
         <v>37</v>
@@ -7824,7 +7867,7 @@
         <v>0.01</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J6">
         <v>0.1</v>
@@ -7844,7 +7887,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>78</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -7857,13 +7900,13 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>0.1</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J7">
         <v>0.1</v>
@@ -7898,7 +7941,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J8">
         <v>0.1</v>
@@ -7930,10 +7973,10 @@
         <v>27</v>
       </c>
       <c r="G9">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J9">
         <v>0.1</v>
@@ -7953,7 +7996,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>79</v>
       </c>
       <c r="C10" s="18" t="s">
@@ -7972,7 +8015,7 @@
         <v>29</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J10">
         <v>0.1</v>
@@ -8007,7 +8050,7 @@
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J11">
         <v>0.1</v>
@@ -8042,7 +8085,7 @@
         <v>29</v>
       </c>
       <c r="I12" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J12">
         <v>0.1</v>
@@ -8061,7 +8104,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="11" t="s">
         <v>80</v>
       </c>
@@ -8103,7 +8146,7 @@
       <c r="P13" s="12"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -8126,7 +8169,7 @@
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J15" s="8">
         <v>0.1</v>
@@ -8148,7 +8191,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="18" t="s">
@@ -8167,7 +8210,7 @@
         <v>0.1</v>
       </c>
       <c r="I16" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J16">
         <v>0.1</v>
@@ -8192,15 +8235,15 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="23">
         <v>0</v>
       </c>
       <c r="G17" s="1"/>
       <c r="I17" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J17">
         <v>0.1</v>
@@ -8229,10 +8272,10 @@
         <v>26</v>
       </c>
       <c r="G18">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="I18" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J18">
         <v>0.1</v>
@@ -8252,7 +8295,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>78</v>
       </c>
       <c r="C19" s="18" t="s">
@@ -8270,8 +8313,11 @@
       <c r="G19">
         <v>0.5</v>
       </c>
+      <c r="H19" t="s">
+        <v>89</v>
+      </c>
       <c r="I19" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J19">
         <v>0.25</v>
@@ -8303,7 +8349,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J20">
         <v>0.25</v>
@@ -8335,7 +8381,7 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J21">
         <v>0.25</v>
@@ -8355,7 +8401,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="18" t="s">
@@ -8374,7 +8420,7 @@
         <v>29</v>
       </c>
       <c r="I22" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J22">
         <v>0.1</v>
@@ -8409,7 +8455,7 @@
         <v>29</v>
       </c>
       <c r="I23" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J23">
         <v>0.1</v>
@@ -8441,7 +8487,7 @@
         <v>29</v>
       </c>
       <c r="I24" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J24">
         <v>0.1</v>
@@ -8460,7 +8506,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="11" t="s">
         <v>80</v>
       </c>
@@ -8502,7 +8548,7 @@
       <c r="P25" s="12"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -8525,7 +8571,7 @@
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="8" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J27" s="8">
         <v>0.1</v>
@@ -8547,7 +8593,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="18" t="s">
@@ -8566,7 +8612,7 @@
         <v>0.1</v>
       </c>
       <c r="I28" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J28">
         <v>0.1</v>
@@ -8598,7 +8644,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J29">
         <v>0.1</v>
@@ -8630,7 +8676,7 @@
         <v>0.1</v>
       </c>
       <c r="I30" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J30">
         <v>0.1</v>
@@ -8650,7 +8696,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="17" t="s">
         <v>78</v>
       </c>
       <c r="C31" s="18" t="s">
@@ -8672,7 +8718,7 @@
         <v>33</v>
       </c>
       <c r="I31" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J31">
         <v>0.1</v>
@@ -8704,7 +8750,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J32">
         <v>0.1</v>
@@ -8739,7 +8785,7 @@
         <v>33</v>
       </c>
       <c r="I33" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J33">
         <v>0.1</v>
@@ -8759,7 +8805,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="17" t="s">
         <v>79</v>
       </c>
       <c r="C34" s="18" t="s">
@@ -8778,7 +8824,7 @@
         <v>29</v>
       </c>
       <c r="I34" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J34">
         <v>0.1</v>
@@ -8803,15 +8849,17 @@
       <c r="D35" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F35" s="1">
-        <v>25</v>
-      </c>
-      <c r="G35" s="1"/>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35">
+        <v>19</v>
+      </c>
+      <c r="G35" t="s">
+        <v>29</v>
+      </c>
       <c r="I35" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J35">
         <v>0.1</v>
@@ -8843,7 +8891,7 @@
         <v>29</v>
       </c>
       <c r="I36" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J36">
         <v>0.1</v>
@@ -8862,7 +8910,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="11" t="s">
         <v>80</v>
       </c>
@@ -8904,7 +8952,7 @@
       <c r="P37" s="12"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="19" t="s">
         <v>34</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -8927,7 +8975,7 @@
       </c>
       <c r="H39" s="8"/>
       <c r="I39" s="8" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J39" s="8">
         <v>0.1</v>
@@ -8968,7 +9016,7 @@
         <v>0.1</v>
       </c>
       <c r="I40" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J40">
         <v>0.1</v>
@@ -9007,7 +9055,7 @@
         <v>0.1</v>
       </c>
       <c r="I41" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J41">
         <v>0.1</v>
@@ -9046,7 +9094,7 @@
         <v>36</v>
       </c>
       <c r="I42" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J42">
         <v>0.1</v>
@@ -9065,7 +9113,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="11" t="s">
         <v>80</v>
       </c>
@@ -9107,7 +9155,7 @@
       <c r="P43" s="12"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -9130,7 +9178,7 @@
       </c>
       <c r="H45" s="8"/>
       <c r="I45" s="8" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J45" s="8">
         <v>0</v>
@@ -9171,7 +9219,7 @@
         <v>0.1</v>
       </c>
       <c r="I46" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -9210,7 +9258,7 @@
         <v>0.1</v>
       </c>
       <c r="I47" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J47">
         <v>0.01</v>
@@ -9249,7 +9297,7 @@
         <v>36</v>
       </c>
       <c r="I48" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="J48">
         <v>0</v>
@@ -9307,7 +9355,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="13" t="s">
         <v>41</v>
       </c>
@@ -9346,6 +9394,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B31:B33"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="A39:A43"/>
     <mergeCell ref="A45:A50"/>
@@ -9362,16 +9420,6 @@
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C16:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -9382,8 +9430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAB967E-925F-4782-9154-55DF58096ABD}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9406,23 +9454,23 @@
       <c r="B1" s="15"/>
       <c r="C1" s="6"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="21" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="H1" s="8"/>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="21" t="s">
         <v>72</v>
       </c>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
       <c r="L1" s="8"/>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
       <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -9472,7 +9520,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -9517,7 +9565,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C4" t="s">
@@ -9624,7 +9672,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>78</v>
       </c>
       <c r="C7" t="s">
@@ -9734,7 +9782,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>79</v>
       </c>
       <c r="C10" t="s">
@@ -9840,7 +9888,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="11" t="s">
         <v>80</v>
       </c>
@@ -9882,7 +9930,7 @@
       <c r="P13" s="12"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -9927,7 +9975,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C16" t="s">
@@ -9952,7 +10000,7 @@
         <v>0.1</v>
       </c>
       <c r="K16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" t="s">
         <v>25</v>
@@ -9973,13 +10021,15 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1"/>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.5</v>
+      </c>
       <c r="I17" t="s">
         <v>21</v>
       </c>
@@ -10032,7 +10082,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>78</v>
       </c>
       <c r="C19" t="s">
@@ -10048,7 +10098,7 @@
         <v>-0.5</v>
       </c>
       <c r="G19">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="I19" t="s">
         <v>21</v>
@@ -10078,13 +10128,15 @@
       <c r="D20" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>28</v>
+      <c r="E20" t="s">
+        <v>22</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1">
+        <v>0.01</v>
+      </c>
       <c r="I20" t="s">
         <v>21</v>
       </c>
@@ -10137,7 +10189,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>79</v>
       </c>
       <c r="C22" t="s">
@@ -10243,7 +10295,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="11" t="s">
         <v>80</v>
       </c>
@@ -10285,7 +10337,7 @@
       <c r="P25" s="12"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -10330,7 +10382,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C28" t="s">
@@ -10367,7 +10419,7 @@
         <v>54</v>
       </c>
       <c r="P28" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -10440,7 +10492,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="17" t="s">
         <v>78</v>
       </c>
       <c r="C31" t="s">
@@ -10477,7 +10529,7 @@
         <v>54</v>
       </c>
       <c r="P31" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -10550,7 +10602,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="17" t="s">
         <v>79</v>
       </c>
       <c r="C34" t="s">
@@ -10656,7 +10708,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="11" t="s">
         <v>80</v>
       </c>
@@ -10699,13 +10751,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="A27:A37"/>
     <mergeCell ref="A15:A25"/>
@@ -10714,6 +10759,13 @@
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Still finalizing the model and writing the report.
</commit_message>
<xml_diff>
--- a/markdown/model_priors.xlsx
+++ b/markdown/model_priors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjjoy\Documents\Rockfish_SF_mortality\RockfishSportMort\markdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A46D1A-ED32-4FCC-8B3E-5DF82E16DD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C348FD-B36E-4535-BEAE-FED5718FF577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3ADC3E42-4C40-4518-B615-B83EB1AEA46F}"/>
+    <workbookView xWindow="-24630" yWindow="0" windowWidth="19860" windowHeight="13710" activeTab="3" xr2:uid="{3ADC3E42-4C40-4518-B615-B83EB1AEA46F}"/>
   </bookViews>
   <sheets>
     <sheet name="Coded" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="92">
   <si>
     <t>Prior</t>
   </si>
@@ -458,6 +458,9 @@
   <si>
     <t>fixed at 0 for NGC, PWSI, PWSO</t>
   </si>
+  <si>
+    <t xml:space="preserve">lower bound -1.5 for CI, SOKO2SAP and northeast </t>
+  </si>
 </sst>
 </file>
 
@@ -554,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -594,10 +597,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -606,13 +612,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7642,7 +7644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EB88A8-0633-428F-BFF5-598E355F3438}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
@@ -7664,23 +7666,23 @@
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="H1" s="8"/>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>86</v>
       </c>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
       <c r="L1" s="8"/>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
       <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -7731,7 +7733,7 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -7775,7 +7777,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -7887,7 +7889,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="19" t="s">
         <v>78</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -7996,7 +7998,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C10" s="18" t="s">
@@ -8104,7 +8106,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="11" t="s">
         <v>80</v>
       </c>
@@ -8146,7 +8148,7 @@
       <c r="P13" s="12"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -8191,7 +8193,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="18" t="s">
@@ -8235,10 +8237,10 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17">
         <v>0</v>
       </c>
       <c r="G17" s="1"/>
@@ -8295,7 +8297,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="19" t="s">
         <v>78</v>
       </c>
       <c r="C19" s="18" t="s">
@@ -8401,7 +8403,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="18" t="s">
@@ -8506,7 +8508,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="11" t="s">
         <v>80</v>
       </c>
@@ -8548,7 +8550,7 @@
       <c r="P25" s="12"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -8593,7 +8595,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="18" t="s">
@@ -8696,7 +8698,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="19" t="s">
         <v>78</v>
       </c>
       <c r="C31" s="18" t="s">
@@ -8805,7 +8807,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C34" s="18" t="s">
@@ -8910,7 +8912,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="11" t="s">
         <v>80</v>
       </c>
@@ -8952,7 +8954,7 @@
       <c r="P37" s="12"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -9113,7 +9115,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="11" t="s">
         <v>80</v>
       </c>
@@ -9155,7 +9157,7 @@
       <c r="P43" s="12"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="20" t="s">
         <v>35</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -9355,7 +9357,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="13" t="s">
         <v>41</v>
       </c>
@@ -9394,16 +9396,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="B31:B33"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="A39:A43"/>
     <mergeCell ref="A45:A50"/>
@@ -9420,6 +9412,16 @@
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C16:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -9430,8 +9432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAB967E-925F-4782-9154-55DF58096ABD}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9454,23 +9456,23 @@
       <c r="B1" s="15"/>
       <c r="C1" s="6"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="H1" s="8"/>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>72</v>
       </c>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
       <c r="L1" s="8"/>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
       <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -9520,7 +9522,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -9565,7 +9567,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C4" t="s">
@@ -9672,7 +9674,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="19" t="s">
         <v>78</v>
       </c>
       <c r="C7" t="s">
@@ -9782,7 +9784,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C10" t="s">
@@ -9888,7 +9890,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="11" t="s">
         <v>80</v>
       </c>
@@ -9930,7 +9932,7 @@
       <c r="P13" s="12"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -9975,7 +9977,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C16" t="s">
@@ -10082,7 +10084,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="19" t="s">
         <v>78</v>
       </c>
       <c r="C19" t="s">
@@ -10189,7 +10191,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C22" t="s">
@@ -10295,7 +10297,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="11" t="s">
         <v>80</v>
       </c>
@@ -10334,10 +10336,12 @@
       <c r="O25" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="P25" s="12"/>
+      <c r="P25" s="12" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="20" t="s">
         <v>61</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -10382,7 +10386,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C28" t="s">
@@ -10492,7 +10496,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="19" t="s">
         <v>78</v>
       </c>
       <c r="C31" t="s">
@@ -10602,7 +10606,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C34" t="s">
@@ -10708,7 +10712,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="11" t="s">
         <v>80</v>
       </c>
@@ -10751,6 +10755,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="A27:A37"/>
     <mergeCell ref="A15:A25"/>
@@ -10759,13 +10770,6 @@
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>